<commit_message>
create excel for CMX and AOB/NOB sims
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMX.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9A5FF6-4D1E-4C2D-9ADC-C131298AAC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39B1B26-1305-4AFF-87FB-C05846E63EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8385" yWindow="-10890" windowWidth="17280" windowHeight="8970" tabRatio="808" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="808" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Discretization" sheetId="27" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Diffusion" sheetId="28" r:id="rId6"/>
     <sheet name="Bacteria" sheetId="25" r:id="rId7"/>
     <sheet name="Solver" sheetId="29" r:id="rId8"/>
-    <sheet name="Influent" sheetId="23" r:id="rId9"/>
-    <sheet name="Initial condition" sheetId="22" r:id="rId10"/>
+    <sheet name="Initial condition" sheetId="22" r:id="rId9"/>
+    <sheet name="Influent" sheetId="23" r:id="rId10"/>
     <sheet name="ThermoParam" sheetId="24" r:id="rId11"/>
     <sheet name="Ks" sheetId="31" r:id="rId12"/>
     <sheet name="Ki" sheetId="32" r:id="rId13"/>
@@ -3501,6 +3501,24 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3534,33 +3552,18 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3570,17 +3573,14 @@
     <xf numFmtId="0" fontId="25" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3597,87 +3597,7 @@
     <cellStyle name="Percent" xfId="8" builtinId="5"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
+  <dxfs count="75">
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -4501,7 +4421,7 @@
       <c r="D1" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="245" t="s">
+      <c r="E1" s="235" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4518,7 +4438,7 @@
       <c r="D2" s="110" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="245"/>
+      <c r="E2" s="235"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -4534,7 +4454,7 @@
       <c r="D3" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="245"/>
+      <c r="E3" s="235"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -4550,7 +4470,7 @@
       <c r="D4" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="245"/>
+      <c r="E4" s="235"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -4565,7 +4485,7 @@
       <c r="D5" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="245"/>
+      <c r="E5" s="235"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -4580,7 +4500,7 @@
       <c r="D6" s="110" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="245"/>
+      <c r="E6" s="235"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
@@ -4595,7 +4515,7 @@
       <c r="D7" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="E7" s="245"/>
+      <c r="E7" s="235"/>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
@@ -4611,7 +4531,7 @@
       <c r="D8" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="246"/>
+      <c r="E8" s="236"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
@@ -4626,7 +4546,7 @@
       <c r="D9" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="247" t="s">
+      <c r="E9" s="237" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4643,7 +4563,7 @@
       <c r="D10" s="110" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="248"/>
+      <c r="E10" s="238"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
@@ -4659,7 +4579,7 @@
       <c r="D11" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="248"/>
+      <c r="E11" s="238"/>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
@@ -4674,7 +4594,7 @@
       <c r="D12" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="248"/>
+      <c r="E12" s="238"/>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
@@ -4689,7 +4609,7 @@
       <c r="D13" s="110" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="248"/>
+      <c r="E13" s="238"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
@@ -4705,7 +4625,7 @@
       <c r="D14" s="111" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="249"/>
+      <c r="E14" s="239"/>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="107" t="s">
@@ -4720,7 +4640,7 @@
       <c r="D15" s="113" t="s">
         <v>157</v>
       </c>
-      <c r="E15" s="247" t="s">
+      <c r="E15" s="237" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4737,7 +4657,7 @@
       <c r="D16" s="114" t="s">
         <v>144</v>
       </c>
-      <c r="E16" s="248"/>
+      <c r="E16" s="238"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="77" t="s">
@@ -4753,7 +4673,7 @@
       <c r="D17" s="114" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="248"/>
+      <c r="E17" s="238"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
@@ -4768,7 +4688,7 @@
       <c r="D18" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="248"/>
+      <c r="E18" s="238"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
@@ -4784,7 +4704,7 @@
       <c r="D19" s="114" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="248"/>
+      <c r="E19" s="238"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
@@ -4799,7 +4719,7 @@
       <c r="D20" s="114" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="248"/>
+      <c r="E20" s="238"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="108" t="s">
@@ -4814,7 +4734,7 @@
       <c r="D21" s="115" t="s">
         <v>155</v>
       </c>
-      <c r="E21" s="248"/>
+      <c r="E21" s="238"/>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
@@ -4829,7 +4749,7 @@
       <c r="D22" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="248"/>
+      <c r="E22" s="238"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
@@ -4844,7 +4764,7 @@
       <c r="D23" s="116" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="248"/>
+      <c r="E23" s="238"/>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
@@ -4859,7 +4779,7 @@
       <c r="D24" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="E24" s="248"/>
+      <c r="E24" s="238"/>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
@@ -4874,7 +4794,7 @@
       <c r="D25" s="116" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="248"/>
+      <c r="E25" s="238"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
@@ -4889,7 +4809,7 @@
       <c r="D26" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="E26" s="248"/>
+      <c r="E26" s="238"/>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="77" t="s">
@@ -4904,7 +4824,7 @@
       <c r="D27" s="116" t="s">
         <v>169</v>
       </c>
-      <c r="E27" s="248"/>
+      <c r="E27" s="238"/>
     </row>
     <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="89" t="s">
@@ -4919,7 +4839,7 @@
       <c r="D28" s="117" t="s">
         <v>170</v>
       </c>
-      <c r="E28" s="249"/>
+      <c r="E28" s="239"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4928,7 +4848,7 @@
     <mergeCell ref="E15:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="90" priority="1">
+    <cfRule type="expression" dxfId="74" priority="1">
       <formula>$B$15 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4943,160 +4863,194 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.44140625" style="62"/>
-    <col min="3" max="3" width="7.5546875" style="62" customWidth="1"/>
-    <col min="4" max="4" width="75.44140625" style="62" customWidth="1"/>
-    <col min="5" max="6" width="11.44140625" style="62"/>
-    <col min="7" max="7" width="12" style="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="62"/>
+    <col min="1" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="4.44140625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="62.5546875" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="131">
-        <f>Influent!B1</f>
+        <f>40/(17*1000)</f>
         <v>2.352941176470588E-3</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="253" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" s="69"/>
+      <c r="D1" s="145" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="254" t="s">
+        <v>232</v>
+      </c>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="131">
-        <f>Influent!B2</f>
         <v>9.9999999999999995E-21</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="253"/>
-      <c r="E2" s="69"/>
+      <c r="D2" s="145" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="254"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <f>Influent!B3</f>
         <v>9.9999999999999995E-21</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="253"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="145" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="254"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="131">
-        <f>Influent!B4</f>
+        <f>6/(32*1000)</f>
         <v>1.875E-4</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="253"/>
-      <c r="E4" s="69"/>
+      <c r="D4" s="145" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="254"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="131">
-        <f>Influent!B5</f>
         <v>1E-3</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="253"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="D5" s="145" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="254"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="69"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="136">
+      <c r="B6" s="131">
         <f>B1/2</f>
         <v>1.176470588235294E-3</v>
       </c>
-      <c r="C6" s="126" t="s">
+      <c r="C6" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="D6" s="145" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="254"/>
+      <c r="F6" s="94"/>
       <c r="G6" s="69"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="152">
+      <c r="B7" s="131">
         <f>B5</f>
         <v>1E-3</v>
       </c>
-      <c r="C7" s="153" t="s">
+      <c r="C7" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="253"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="146"/>
-      <c r="G7" s="146"/>
-      <c r="H7" s="147"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="69"/>
-      <c r="F8" s="148"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="150"/>
-      <c r="I8" s="148"/>
-      <c r="J8" s="147"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="94"/>
+      <c r="D7" s="145" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="254"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:D7"/>
+    <mergeCell ref="E1:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5457,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="252" t="s">
+      <c r="I13" s="254" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5482,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="252"/>
+      <c r="I14" s="254"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
@@ -5505,7 +5459,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="252"/>
+      <c r="I15" s="254"/>
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
@@ -5528,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="252"/>
+      <c r="I16" s="254"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
@@ -5551,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="252"/>
+      <c r="I17" s="254"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="108" t="s">
@@ -5574,7 +5528,7 @@
       </c>
       <c r="F18" s="71"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="252"/>
+      <c r="I18" s="254"/>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="151" t="s">
@@ -5598,7 +5552,7 @@
       </c>
       <c r="F19" s="71"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="252"/>
+      <c r="I19" s="254"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="151" t="s">
@@ -5622,7 +5576,7 @@
       </c>
       <c r="F20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="252"/>
+      <c r="I20" s="254"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="160" t="s">
@@ -5646,7 +5600,7 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="252"/>
+      <c r="I21" s="254"/>
     </row>
     <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="161" t="s">
@@ -5669,17 +5623,17 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="252"/>
+      <c r="I22" s="254"/>
     </row>
     <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="254" t="s">
+      <c r="A23" s="255" t="s">
         <v>238</v>
       </c>
-      <c r="B23" s="255"/>
-      <c r="C23" s="255"/>
-      <c r="D23" s="255"/>
-      <c r="E23" s="255"/>
-      <c r="F23" s="256"/>
+      <c r="B23" s="256"/>
+      <c r="C23" s="256"/>
+      <c r="D23" s="256"/>
+      <c r="E23" s="256"/>
+      <c r="F23" s="257"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -5700,7 +5654,7 @@
       <c r="F24" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="252" t="s">
+      <c r="I24" s="254" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5723,7 +5677,7 @@
       <c r="F25" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="252"/>
+      <c r="I25" s="254"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
@@ -5744,7 +5698,7 @@
       <c r="F26" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="252"/>
+      <c r="I26" s="254"/>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
@@ -5765,7 +5719,7 @@
       <c r="F27" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="252"/>
+      <c r="I27" s="254"/>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
@@ -5786,7 +5740,7 @@
       <c r="F28" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="252"/>
+      <c r="I28" s="254"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
@@ -5807,7 +5761,7 @@
       <c r="F29" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="252"/>
+      <c r="I29" s="254"/>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="151" t="s">
@@ -5828,7 +5782,7 @@
       <c r="F30" s="192" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="252"/>
+      <c r="I30" s="254"/>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="151" t="s">
@@ -5849,7 +5803,7 @@
       <c r="F31" s="190" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="252"/>
+      <c r="I31" s="254"/>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="160" t="s">
@@ -5870,7 +5824,7 @@
       <c r="F32" s="186" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="252"/>
+      <c r="I32" s="254"/>
     </row>
     <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="161" t="s">
@@ -5891,7 +5845,7 @@
       <c r="F33" s="175" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="252"/>
+      <c r="I33" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5901,15 +5855,15 @@
     <mergeCell ref="I24:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:F11 B24:F33 B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="containsText" dxfId="60" priority="54" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="55" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="43" priority="55" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5947,7 +5901,7 @@
       <c r="D1" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="244" t="s">
+      <c r="E1" s="250" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5964,7 +5918,7 @@
       <c r="D2" s="157">
         <v>3.5937500000000001E-6</v>
       </c>
-      <c r="E2" s="244"/>
+      <c r="E2" s="250"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5979,7 +5933,7 @@
       <c r="D3" s="157">
         <v>7.8125000000000002E-6</v>
       </c>
-      <c r="E3" s="244"/>
+      <c r="E3" s="250"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
@@ -5994,7 +5948,7 @@
       <c r="D4" s="157">
         <v>2.5937500000000004E-6</v>
       </c>
-      <c r="E4" s="244"/>
+      <c r="E4" s="250"/>
     </row>
     <row r="5" spans="1:5" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
@@ -6009,7 +5963,7 @@
       <c r="D5" s="157">
         <v>0</v>
       </c>
-      <c r="E5" s="244"/>
+      <c r="E5" s="250"/>
     </row>
     <row r="6" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="219"/>
@@ -6023,7 +5977,7 @@
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <conditionalFormatting sqref="B2:D7">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6058,7 +6012,7 @@
       <c r="D1" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="244" t="s">
+      <c r="E1" s="250" t="s">
         <v>249</v>
       </c>
     </row>
@@ -6075,7 +6029,7 @@
       <c r="D2" s="157">
         <v>0</v>
       </c>
-      <c r="E2" s="244"/>
+      <c r="E2" s="250"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -6090,7 +6044,7 @@
       <c r="D3" s="157">
         <v>0</v>
       </c>
-      <c r="E3" s="244"/>
+      <c r="E3" s="250"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
@@ -6105,7 +6059,7 @@
       <c r="D4" s="157">
         <v>0</v>
       </c>
-      <c r="E4" s="244"/>
+      <c r="E4" s="250"/>
     </row>
     <row r="5" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
@@ -6120,14 +6074,14 @@
       <c r="D5" s="157">
         <v>3.1250000000000003E-7</v>
       </c>
-      <c r="E5" s="244"/>
+      <c r="E5" s="250"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:D5">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6180,7 +6134,7 @@
       </c>
       <c r="D2" s="159"/>
       <c r="E2" s="159"/>
-      <c r="F2" s="260" t="s">
+      <c r="F2" s="234" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6196,7 +6150,7 @@
       </c>
       <c r="D3" s="159"/>
       <c r="E3" s="159"/>
-      <c r="F3" s="260"/>
+      <c r="F3" s="234"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
@@ -6210,7 +6164,7 @@
       </c>
       <c r="D4" s="159"/>
       <c r="E4" s="159"/>
-      <c r="F4" s="260"/>
+      <c r="F4" s="234"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
@@ -6225,7 +6179,7 @@
       </c>
       <c r="D5" s="159"/>
       <c r="E5" s="159"/>
-      <c r="F5" s="260"/>
+      <c r="F5" s="234"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6260,26 +6214,26 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
-      <c r="B1" s="259" t="s">
+      <c r="B1" s="258" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="257"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="259" t="s">
+      <c r="C1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="258" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="257"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="259" t="s">
+      <c r="F1" s="259"/>
+      <c r="G1" s="260"/>
+      <c r="H1" s="258" t="s">
         <v>252</v>
       </c>
-      <c r="I1" s="257"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="257" t="s">
+      <c r="I1" s="259"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="259" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="257"/>
-      <c r="M1" s="258"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="260"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
@@ -6738,187 +6692,187 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:B12 E3:F7 E10:G12 J10:J12">
-    <cfRule type="cellIs" dxfId="55" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12">
-    <cfRule type="cellIs" dxfId="53" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B7">
-    <cfRule type="cellIs" dxfId="51" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="50" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D7">
-    <cfRule type="cellIs" dxfId="49" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="cellIs" dxfId="48" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="46" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I7 H10:I12">
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L7 K10:L12">
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M12">
-    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K7">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M7">
-    <cfRule type="cellIs" dxfId="24" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7036,25 +6990,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="89" priority="6">
+    <cfRule type="expression" dxfId="73" priority="6">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="88" priority="4" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="5" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="85" priority="1">
+    <cfRule type="expression" dxfId="69" priority="1">
       <formula>$B$11&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7109,30 +7063,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="S2" s="234" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="234"/>
-      <c r="U2" s="234"/>
-      <c r="V2" s="234"/>
-      <c r="W2" s="234" t="s">
+      <c r="S2" s="240" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="240"/>
+      <c r="U2" s="240"/>
+      <c r="V2" s="240"/>
+      <c r="W2" s="240" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="234"/>
-      <c r="Y2" s="234"/>
-      <c r="Z2" s="234"/>
-      <c r="AA2" s="234" t="s">
+      <c r="X2" s="240"/>
+      <c r="Y2" s="240"/>
+      <c r="Z2" s="240"/>
+      <c r="AA2" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="234"/>
-      <c r="AC2" s="234"/>
-      <c r="AD2" s="234"/>
-      <c r="AE2" s="234" t="s">
+      <c r="AB2" s="240"/>
+      <c r="AC2" s="240"/>
+      <c r="AD2" s="240"/>
+      <c r="AE2" s="240" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="234"/>
-      <c r="AG2" s="234"/>
-      <c r="AH2" s="234"/>
+      <c r="AF2" s="240"/>
+      <c r="AG2" s="240"/>
+      <c r="AH2" s="240"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -8585,10 +8539,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="235" t="s">
+      <c r="J17" s="241" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="238" t="s">
+      <c r="K17" s="244" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8688,8 +8642,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="236"/>
-      <c r="K18" s="239"/>
+      <c r="J18" s="242"/>
+      <c r="K18" s="245"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8787,8 +8741,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="236"/>
-      <c r="K19" s="239"/>
+      <c r="J19" s="242"/>
+      <c r="K19" s="245"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -8868,8 +8822,8 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="236"/>
-      <c r="K20" s="239"/>
+      <c r="J20" s="242"/>
+      <c r="K20" s="245"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -8950,8 +8904,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="236"/>
-      <c r="K21" s="239"/>
+      <c r="J21" s="242"/>
+      <c r="K21" s="245"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -9032,8 +8986,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="236"/>
-      <c r="K22" s="239"/>
+      <c r="J22" s="242"/>
+      <c r="K22" s="245"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -9114,8 +9068,8 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="236"/>
-      <c r="K23" s="239"/>
+      <c r="J23" s="242"/>
+      <c r="K23" s="245"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -9196,8 +9150,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="236"/>
-      <c r="K24" s="239"/>
+      <c r="J24" s="242"/>
+      <c r="K24" s="245"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -9218,8 +9172,8 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="236"/>
-      <c r="K25" s="239"/>
+      <c r="J25" s="242"/>
+      <c r="K25" s="245"/>
     </row>
     <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
@@ -9228,14 +9182,14 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="236"/>
-      <c r="K26" s="239"/>
-      <c r="N26" s="241" t="s">
+      <c r="J26" s="242"/>
+      <c r="K26" s="245"/>
+      <c r="N26" s="247" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="242"/>
-      <c r="P26" s="242"/>
-      <c r="Q26" s="243"/>
+      <c r="O26" s="248"/>
+      <c r="P26" s="248"/>
+      <c r="Q26" s="249"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -9311,14 +9265,14 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="236"/>
-      <c r="K27" s="239"/>
-      <c r="N27" s="241" t="s">
+      <c r="J27" s="242"/>
+      <c r="K27" s="245"/>
+      <c r="N27" s="247" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="242"/>
-      <c r="P27" s="242"/>
-      <c r="Q27" s="243"/>
+      <c r="O27" s="248"/>
+      <c r="P27" s="248"/>
+      <c r="Q27" s="249"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -9394,8 +9348,8 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="236"/>
-      <c r="K28" s="239"/>
+      <c r="J28" s="242"/>
+      <c r="K28" s="245"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
@@ -9407,24 +9361,24 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="236"/>
-      <c r="K29" s="239"/>
+      <c r="J29" s="242"/>
+      <c r="K29" s="245"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J30" s="236"/>
-      <c r="K30" s="239"/>
+      <c r="J30" s="242"/>
+      <c r="K30" s="245"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J31" s="236"/>
-      <c r="K31" s="239"/>
+      <c r="J31" s="242"/>
+      <c r="K31" s="245"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J32" s="236"/>
-      <c r="K32" s="239"/>
+      <c r="J32" s="242"/>
+      <c r="K32" s="245"/>
     </row>
     <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J33" s="237"/>
-      <c r="K33" s="240"/>
+      <c r="J33" s="243"/>
+      <c r="K33" s="246"/>
     </row>
     <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
@@ -9536,82 +9490,82 @@
     <mergeCell ref="N27:Q27"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:AB7 AD5:AD7 AD9:AD16 S9:AB16">
-    <cfRule type="cellIs" dxfId="84" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:AD23">
-    <cfRule type="cellIs" dxfId="83" priority="19" operator="notBetween">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AB8 AD8">
-    <cfRule type="cellIs" dxfId="81" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5:AC7 AC9:AC16">
-    <cfRule type="cellIs" dxfId="80" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="79" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5:AF7 AE9:AF16 AH9:AI16 AH5:AJ5 AH6:AI7 AJ6:AJ16 AH4">
-    <cfRule type="cellIs" dxfId="77" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AJ23">
-    <cfRule type="cellIs" dxfId="76" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="60" priority="9" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="10" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8 AH8:AI8">
-    <cfRule type="cellIs" dxfId="74" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5:AG7 AG9:AG16">
-    <cfRule type="cellIs" dxfId="73" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4 S4:AB4">
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4 AI4">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9644,7 +9598,7 @@
         <f>Discretization!B15</f>
         <v>1</v>
       </c>
-      <c r="C1" s="244" t="s">
+      <c r="C1" s="250" t="s">
         <v>264</v>
       </c>
     </row>
@@ -9657,7 +9611,7 @@
         <f>Parameters!B2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="244"/>
+      <c r="C2" s="250"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
@@ -9668,7 +9622,7 @@
         <f>Bacteria!B6</f>
         <v>granule</v>
       </c>
-      <c r="C3" s="244"/>
+      <c r="C3" s="250"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
@@ -9679,7 +9633,7 @@
         <f>Bacteria!B12</f>
         <v>1</v>
       </c>
-      <c r="C4" s="244"/>
+      <c r="C4" s="250"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
@@ -9690,7 +9644,7 @@
         <f>Bacteria!B13</f>
         <v>mechanistic</v>
       </c>
-      <c r="C5" s="244"/>
+      <c r="C5" s="250"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
@@ -9701,7 +9655,7 @@
         <f>Solver!B4</f>
         <v>1</v>
       </c>
-      <c r="C6" s="244"/>
+      <c r="C6" s="250"/>
     </row>
     <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
@@ -9712,7 +9666,7 @@
         <f>Solver!B2</f>
         <v>1</v>
       </c>
-      <c r="C7" s="244"/>
+      <c r="C7" s="250"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="str">
@@ -9723,7 +9677,7 @@
         <f>Solver!B5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="244"/>
+      <c r="C8" s="250"/>
     </row>
     <row r="9" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="219"/>
@@ -10029,12 +9983,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="68" priority="3">
+    <cfRule type="expression" dxfId="52" priority="3">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="67" priority="1">
+    <cfRule type="expression" dxfId="51" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10082,7 +10036,7 @@
       <c r="D1" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="250" t="s">
+      <c r="E1" s="251" t="s">
         <v>186</v>
       </c>
     </row>
@@ -10100,7 +10054,7 @@
       <c r="D2" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="250"/>
+      <c r="E2" s="251"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -10116,7 +10070,7 @@
       <c r="D3" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="250"/>
+      <c r="E3" s="251"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -10132,7 +10086,7 @@
       <c r="D4" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="250"/>
+      <c r="E4" s="251"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -10148,7 +10102,7 @@
       <c r="D5" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="250"/>
+      <c r="E5" s="251"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -10164,7 +10118,7 @@
       <c r="D6" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="250"/>
+      <c r="E6" s="251"/>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
@@ -10180,7 +10134,7 @@
       <c r="D7" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E7" s="251"/>
+      <c r="E7" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10195,7 +10149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -10302,8 +10256,8 @@
         <v>194</v>
       </c>
       <c r="B7" s="131">
-        <f>50*10^(-6)</f>
-        <v>4.9999999999999996E-5</v>
+        <f>75*10^(-6)</f>
+        <v>7.4999999999999993E-5</v>
       </c>
       <c r="C7" s="90" t="s">
         <v>94</v>
@@ -10318,7 +10272,7 @@
       </c>
       <c r="B8" s="231">
         <f>_xlfn.CEILING.MATH(B7^2 / (0.8*B3 * B11)^2 * 0.75)</f>
-        <v>1303</v>
+        <v>2930</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>97</v>
@@ -10403,7 +10357,7 @@
         <v>208</v>
       </c>
       <c r="B14" s="132">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C14" s="90" t="s">
         <v>209</v>
@@ -10450,22 +10404,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A14:D14">
-    <cfRule type="expression" dxfId="66" priority="4">
+    <cfRule type="expression" dxfId="50" priority="4">
       <formula>$B$13&lt;&gt;"mechanistic"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:D15">
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="49" priority="3">
       <formula>$B$13&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D9">
-    <cfRule type="expression" dxfId="64" priority="1">
+    <cfRule type="expression" dxfId="48" priority="1">
       <formula>$B$6 = "granule"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:D8">
-    <cfRule type="expression" dxfId="63" priority="2">
+    <cfRule type="expression" dxfId="47" priority="2">
       <formula>$B$6 ="suspension"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10669,12 +10623,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="62" priority="2">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>$B$2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:D12">
-    <cfRule type="expression" dxfId="61" priority="1">
+    <cfRule type="expression" dxfId="45" priority="1">
       <formula>$B$11=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10695,194 +10649,156 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="62"/>
-    <col min="4" max="4" width="4.44140625" style="62" customWidth="1"/>
-    <col min="5" max="5" width="62.5546875" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="62"/>
+    <col min="1" max="2" width="11.44140625" style="62"/>
+    <col min="3" max="3" width="7.5546875" style="62" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="62" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" style="62"/>
+    <col min="7" max="7" width="12" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="131">
-        <f>40/(17*1000)</f>
-        <v>2.352941176470588E-3</v>
+        <v>1E-10</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="145" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="252" t="s">
-        <v>232</v>
-      </c>
+      <c r="D1" s="253" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="69"/>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="131">
-        <v>9.9999999999999995E-21</v>
+        <v>1E-10</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="145" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="252"/>
+      <c r="D2" s="253"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <v>9.9999999999999995E-21</v>
+        <v>1E-10</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="145" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="252"/>
+      <c r="D3" s="253"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="131">
-        <f>6/(32*1000)</f>
-        <v>1.875E-4</v>
+        <v>1E-10</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="145" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="252"/>
+      <c r="D4" s="253"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="131">
+        <f>Influent!B5</f>
         <v>1E-3</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="145" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="252"/>
-      <c r="F5" s="94"/>
+      <c r="D5" s="253"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="131">
+      <c r="B6" s="136">
         <f>B1/2</f>
-        <v>1.176470588235294E-3</v>
-      </c>
-      <c r="C6" s="90" t="s">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="C6" s="126" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="145" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="252"/>
-      <c r="F6" s="94"/>
+      <c r="D6" s="253"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="131">
+      <c r="B7" s="152">
         <f>B5</f>
         <v>1E-3</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="153" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="145" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="252"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="70"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
+      <c r="D7" s="253"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="69"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="149"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="147"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:E7"/>
+    <mergeCell ref="D1:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update excels with Vr calculation
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMX.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMX.xlsx
@@ -1,40 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bestanden\Cloud Storage\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3DEA75-BA06-46CD-B0A2-10CBF6269B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F79126-7EDF-4C78-9134-95FBD8379C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="808" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="8124" windowHeight="8964" tabRatio="808" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Discretization" sheetId="27" r:id="rId1"/>
-    <sheet name="Information" sheetId="30" r:id="rId2"/>
-    <sheet name="Reactions" sheetId="18" state="hidden" r:id="rId3"/>
-    <sheet name="Settings" sheetId="34" r:id="rId4"/>
+    <sheet name="Information" sheetId="30" r:id="rId1"/>
+    <sheet name="Reactions" sheetId="18" state="hidden" r:id="rId2"/>
+    <sheet name="Settings" sheetId="34" r:id="rId3"/>
+    <sheet name="Discretization" sheetId="27" r:id="rId4"/>
     <sheet name="Parameters" sheetId="26" r:id="rId5"/>
     <sheet name="Diffusion" sheetId="28" r:id="rId6"/>
     <sheet name="Bacteria" sheetId="25" r:id="rId7"/>
     <sheet name="Solver" sheetId="29" r:id="rId8"/>
-    <sheet name="Initial condition" sheetId="22" r:id="rId9"/>
-    <sheet name="Influent" sheetId="23" r:id="rId10"/>
+    <sheet name="Influent" sheetId="23" r:id="rId9"/>
+    <sheet name="Initial condition" sheetId="22" r:id="rId10"/>
     <sheet name="ThermoParam" sheetId="24" r:id="rId11"/>
     <sheet name="Ks" sheetId="31" r:id="rId12"/>
     <sheet name="Ki" sheetId="32" r:id="rId13"/>
     <sheet name="Yield" sheetId="33" r:id="rId14"/>
     <sheet name="ReactionMatrix" sheetId="21" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -43,6 +45,24 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={873F5D62-7A36-441D-909B-5D8DF0BCC1F4}</author>
+  </authors>
+  <commentList>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{873F5D62-7A36-441D-909B-5D8DF0BCC1F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lemaire2008 -&gt; order of magnitude 30-80 g/L for synthetic feed, 150 g/L in their experiment</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Chiel</author>
@@ -150,7 +170,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={FAFA8C7C-6800-4018-947D-B9F524B630BA}</author>
@@ -158,16 +178,10 @@
   <commentList>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{FAFA8C7C-6800-4018-947D-B9F524B630BA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     From [Strous1998]</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -175,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="289">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1160,9 +1174,6 @@
     <t>pH value at which to control the bulk liquid</t>
   </si>
   <si>
-    <t>CALCULATED Representative volume of the reactor that is modelled in the simulation domain</t>
-  </si>
-  <si>
     <t>Diffusivity</t>
   </si>
   <si>
@@ -1452,6 +1463,30 @@
   </si>
   <si>
     <t>mechanistic</t>
+  </si>
+  <si>
+    <t>CALCULATED Representative volume of the reactor that is modelled in the simulation domain. Calculated using the average expected granule radius and the density of biomass in the reactor and the density per granule</t>
+  </si>
+  <si>
+    <t>Average expected granule radius</t>
+  </si>
+  <si>
+    <t>Average expected radius of all granules</t>
+  </si>
+  <si>
+    <t>density granule</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
+  <si>
+    <t>How dense are the granules</t>
+  </si>
+  <si>
+    <t>density reactor</t>
+  </si>
+  <si>
+    <t>How much biomass (at most) is in the reactor</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1503,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1743,6 +1778,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2894,7 +2935,7 @@
     <xf numFmtId="0" fontId="35" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -3508,6 +3549,39 @@
     <xf numFmtId="171" fontId="0" fillId="11" borderId="41" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3523,51 +3597,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3584,6 +3625,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3919,6 +3963,17 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
     </dxf>
@@ -4038,17 +4093,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4064,6 +4108,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Chiel van Amstel" id="{969302A7-3B3A-4079-852A-4AE1C0564048}" userId="Chiel van Amstel" providerId="None"/>
   <person displayName="Eloi Martínez-Rabert (PGR)" id="{5CC223E8-22CF-48C3-ABCE-0A00391E726E}" userId="S::2424069M@student.gla.ac.uk::cb616271-4a7a-48f5-8972-853218eda004" providerId="AD"/>
 </personList>
 </file>
@@ -4389,6 +4434,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B11" dT="2021-12-16T15:08:36.62" personId="{969302A7-3B3A-4079-852A-4AE1C0564048}" id="{873F5D62-7A36-441D-909B-5D8DF0BCC1F4}">
+    <text>Lemaire2008 -&gt; order of magnitude 30-80 g/L for synthetic feed, 150 g/L in their experiment</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="B5" dT="2021-05-06T16:02:09.77" personId="{5CC223E8-22CF-48C3-ABCE-0A00391E726E}" id="{FAFA8C7C-6800-4018-947D-B9F524B630BA}">
     <text>From [Strous1998]</text>
   </threadedComment>
@@ -4396,665 +4449,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="66.85546875" style="62" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="122">
-        <v>257</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="235" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="133">
-        <v>257</v>
-      </c>
-      <c r="C2" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="110" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="235"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="99">
-        <f>B5*B1*1000000</f>
-        <v>1028</v>
-      </c>
-      <c r="C3" s="90" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="110" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="235"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="99">
-        <f>B6*B2*1000000</f>
-        <v>1028</v>
-      </c>
-      <c r="C4" s="90" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="110" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="235"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="103">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C5" s="90" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="110" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="235"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="103">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C6" s="90" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="110" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="235"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="103">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="C7" s="90" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="110" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="235"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="89" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="104">
-        <f>5*10^(-6)</f>
-        <v>4.9999999999999996E-6</v>
-      </c>
-      <c r="C8" s="92" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="111" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="236"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="105">
-        <v>6500</v>
-      </c>
-      <c r="C9" s="91" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="112" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="237" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="102">
-        <v>0.2</v>
-      </c>
-      <c r="C10" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="110" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="238"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="98">
-        <f>$B$5^2 * B10 / MAX(Diffusion!$B:$B)</f>
-        <v>6.0468631897203323E-7</v>
-      </c>
-      <c r="C11" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="110" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="238"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="102">
-        <v>0.5</v>
-      </c>
-      <c r="C12" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="110" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="238"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="106">
-        <v>24</v>
-      </c>
-      <c r="C13" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="110" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" s="238"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="89" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="100">
-        <f>24*7</f>
-        <v>168</v>
-      </c>
-      <c r="C14" s="124" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="111" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="239"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="107" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" s="134" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="125" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="113" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="237" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="B16" s="102">
-        <v>0.01</v>
-      </c>
-      <c r="C16" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="114" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="238"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="98">
-        <f>$B$5^2 * B16 / MAX(Diffusion!$B:$B)</f>
-        <v>3.0234315948601663E-8</v>
-      </c>
-      <c r="C17" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="114" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="238"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="102">
-        <v>0.5</v>
-      </c>
-      <c r="C18" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="114" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="238"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="98">
-        <f>$B$5^2 * B18 / MAX(Diffusion!$B:$B)</f>
-        <v>1.511715797430083E-6</v>
-      </c>
-      <c r="C19" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="114" t="s">
-        <v>148</v>
-      </c>
-      <c r="E19" s="238"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20" s="102">
-        <v>0.05</v>
-      </c>
-      <c r="C20" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="114" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="238"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="108" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="109">
-        <v>1</v>
-      </c>
-      <c r="C21" s="126" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="115" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" s="238"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
-        <v>158</v>
-      </c>
-      <c r="B22" s="102">
-        <v>3</v>
-      </c>
-      <c r="C22" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" s="238"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="B23" s="102">
-        <v>500</v>
-      </c>
-      <c r="C23" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="116" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="238"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="77" t="s">
-        <v>159</v>
-      </c>
-      <c r="B24" s="102">
-        <v>200</v>
-      </c>
-      <c r="C24" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="116" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="238"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="77" t="s">
-        <v>160</v>
-      </c>
-      <c r="B25" s="102">
-        <v>40</v>
-      </c>
-      <c r="C25" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="116" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="238"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="77" t="s">
-        <v>168</v>
-      </c>
-      <c r="B26" s="119">
-        <v>0.2</v>
-      </c>
-      <c r="C26" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="116" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" s="238"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="118">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C27" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="116" t="s">
-        <v>169</v>
-      </c>
-      <c r="E27" s="238"/>
-    </row>
-    <row r="28" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="89" t="s">
-        <v>163</v>
-      </c>
-      <c r="B28" s="120">
-        <v>0.02</v>
-      </c>
-      <c r="C28" s="124" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="117" t="s">
-        <v>170</v>
-      </c>
-      <c r="E28" s="239"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="A9" s="227" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="228" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="226" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="225" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="221" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="220" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="222" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="223" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="224" t="s">
+        <v>272</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E1:E8"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="E15:E28"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="74" priority="1">
-      <formula>$B$15 = FALSE</formula>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="expression" dxfId="74" priority="6">
+      <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{B02285CC-B93F-41B6-9F0B-F56D7F2E2904}">
-      <formula1>"TRUE, FALSE"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="5" operator="containsText" text="Inf">
+      <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="70" priority="1">
+      <formula>$B$11&lt;&gt;"naive"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="4.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="62.5703125" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="2" width="11.44140625" style="62"/>
+    <col min="3" max="3" width="7.5546875" style="62" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="62" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" style="62"/>
+    <col min="7" max="7" width="12" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="131">
-        <f>40/(17*1000)</f>
-        <v>2.352941176470588E-3</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="254" t="s">
-        <v>232</v>
-      </c>
+      <c r="D1" s="254" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="69"/>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="131">
-        <v>9.9999999999999995E-21</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="254"/>
+      <c r="D2" s="254"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <v>9.9999999999999995E-21</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="254"/>
+      <c r="D3" s="254"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="131">
-        <f>6/(32*1000)</f>
+        <f>Influent!B4</f>
         <v>1.875E-4</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="254"/>
+      <c r="D4" s="254"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="131">
+        <f>Influent!B5</f>
         <v>1E-3</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="254"/>
-      <c r="F5" s="94"/>
+      <c r="D5" s="254"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="77" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="131">
+      <c r="B6" s="135">
         <f>B1/2</f>
-        <v>1.176470588235294E-3</v>
-      </c>
-      <c r="C6" s="90" t="s">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="C6" s="126" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="254"/>
-      <c r="F6" s="94"/>
+      <c r="D6" s="254"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="77" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="131">
+      <c r="B7" s="151">
         <f>B5</f>
         <v>1E-3</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="144" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="254"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="70"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="69"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
+      <c r="D7" s="254"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="69"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="148"/>
+      <c r="H8" s="149"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="146"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:E7"/>
+    <mergeCell ref="D1:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5065,43 +4731,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="6" width="14.28515625" style="75" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="71" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="72" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="6" width="14.33203125" style="75" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="71" customWidth="1"/>
+    <col min="8" max="8" width="3.5546875" style="72" customWidth="1"/>
+    <col min="9" max="9" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="161" t="s">
         <v>91</v>
       </c>
       <c r="B1" s="162" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C1" s="162" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="163" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="163" t="s">
+      <c r="E1" s="162" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="162" t="s">
+      <c r="F1" s="163" t="s">
         <v>235</v>
       </c>
-      <c r="F1" s="163" t="s">
-        <v>236</v>
-      </c>
       <c r="G1" s="163" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>74</v>
       </c>
@@ -5126,11 +4792,11 @@
       <c r="H2" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="253" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I2" s="254" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>75</v>
       </c>
@@ -5155,9 +4821,9 @@
       <c r="H3" s="165" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="253"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I3" s="254"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>80</v>
       </c>
@@ -5182,9 +4848,9 @@
       <c r="H4" s="165" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="253"/>
-    </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I4" s="254"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>81</v>
       </c>
@@ -5209,9 +4875,9 @@
       <c r="H5" s="165" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="253"/>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I5" s="254"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>82</v>
       </c>
@@ -5237,9 +4903,9 @@
       <c r="H6" s="165" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="253"/>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I6" s="254"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>83</v>
       </c>
@@ -5266,9 +4932,9 @@
       <c r="H7" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="253"/>
-    </row>
-    <row r="8" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I7" s="254"/>
+    </row>
+    <row r="8" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="150" t="s">
         <v>84</v>
       </c>
@@ -5293,9 +4959,9 @@
       <c r="H8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="253"/>
-    </row>
-    <row r="9" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I8" s="254"/>
+    </row>
+    <row r="9" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
         <v>85</v>
       </c>
@@ -5320,9 +4986,9 @@
       <c r="H9" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="253"/>
-    </row>
-    <row r="10" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I9" s="254"/>
+    </row>
+    <row r="10" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="159" t="s">
         <v>86</v>
       </c>
@@ -5347,9 +5013,9 @@
       <c r="H10" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="253"/>
-    </row>
-    <row r="11" spans="1:9" s="71" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="254"/>
+    </row>
+    <row r="11" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="160" t="s">
         <v>18</v>
       </c>
@@ -5374,27 +5040,27 @@
       <c r="H11" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="253"/>
-    </row>
-    <row r="12" spans="1:9" s="71" customFormat="1" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="254"/>
+    </row>
+    <row r="12" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="161" t="s">
         <v>91</v>
       </c>
       <c r="B12" s="166" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="166" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="166" t="s">
+      <c r="D12" s="167" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="167" t="s">
+      <c r="E12" s="166" t="s">
         <v>241</v>
       </c>
-      <c r="E12" s="166" t="s">
-        <v>242</v>
-      </c>
       <c r="H12" s="72"/>
     </row>
-    <row r="13" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
         <v>74</v>
       </c>
@@ -5415,11 +5081,11 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="254" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I13" s="253" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>75</v>
       </c>
@@ -5440,9 +5106,9 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="254"/>
-    </row>
-    <row r="15" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I14" s="253"/>
+    </row>
+    <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>80</v>
       </c>
@@ -5463,9 +5129,9 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="254"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I15" s="253"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
         <v>81</v>
       </c>
@@ -5486,9 +5152,9 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="254"/>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I16" s="253"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>82</v>
       </c>
@@ -5509,9 +5175,9 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="254"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I17" s="253"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="108" t="s">
         <v>83</v>
       </c>
@@ -5532,9 +5198,9 @@
       </c>
       <c r="F18" s="71"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="254"/>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I18" s="253"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="150" t="s">
         <v>84</v>
       </c>
@@ -5556,9 +5222,9 @@
       </c>
       <c r="F19" s="71"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="254"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I19" s="253"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="150" t="s">
         <v>85</v>
       </c>
@@ -5580,9 +5246,9 @@
       </c>
       <c r="F20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="254"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I20" s="253"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="159" t="s">
         <v>86</v>
       </c>
@@ -5604,9 +5270,9 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="254"/>
-    </row>
-    <row r="22" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="253"/>
+    </row>
+    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="160" t="s">
         <v>18</v>
       </c>
@@ -5627,11 +5293,11 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="254"/>
-    </row>
-    <row r="23" spans="1:9" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="253"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="255" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="256"/>
       <c r="C23" s="256"/>
@@ -5639,7 +5305,7 @@
       <c r="E23" s="256"/>
       <c r="F23" s="257"/>
     </row>
-    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
         <v>74</v>
       </c>
@@ -5658,11 +5324,11 @@
       <c r="F24" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="254" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I24" s="253" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
         <v>75</v>
       </c>
@@ -5681,9 +5347,9 @@
       <c r="F25" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="254"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I25" s="253"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
         <v>80</v>
       </c>
@@ -5702,9 +5368,9 @@
       <c r="F26" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="254"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I26" s="253"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>81</v>
       </c>
@@ -5723,9 +5389,9 @@
       <c r="F27" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="254"/>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I27" s="253"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>82</v>
       </c>
@@ -5744,9 +5410,9 @@
       <c r="F28" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="254"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I28" s="253"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
         <v>83</v>
       </c>
@@ -5765,9 +5431,9 @@
       <c r="F29" s="187" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="254"/>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I29" s="253"/>
+    </row>
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="150" t="s">
         <v>84</v>
       </c>
@@ -5786,9 +5452,9 @@
       <c r="F30" s="191" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="254"/>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I30" s="253"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="150" t="s">
         <v>85</v>
       </c>
@@ -5807,9 +5473,9 @@
       <c r="F31" s="189" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="254"/>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I31" s="253"/>
+    </row>
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="159" t="s">
         <v>86</v>
       </c>
@@ -5828,9 +5494,9 @@
       <c r="F32" s="185" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="254"/>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="253"/>
+    </row>
+    <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="160" t="s">
         <v>18</v>
       </c>
@@ -5849,7 +5515,7 @@
       <c r="F33" s="174" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="254"/>
+      <c r="I33" s="253"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5885,16 +5551,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="155" t="s">
         <v>74</v>
@@ -5905,11 +5571,11 @@
       <c r="D1" s="155" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="250" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="245" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
@@ -5922,11 +5588,11 @@
       <c r="D2" s="156">
         <v>3.5937500000000001E-6</v>
       </c>
-      <c r="E2" s="250"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="245"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="156">
         <v>0</v>
@@ -5937,11 +5603,11 @@
       <c r="D3" s="156">
         <v>7.8125000000000002E-6</v>
       </c>
-      <c r="E3" s="250"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="245"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="156">
         <v>0</v>
@@ -5952,9 +5618,9 @@
       <c r="D4" s="156">
         <v>2.5937500000000004E-6</v>
       </c>
-      <c r="E4" s="250"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="245"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
         <v>76</v>
       </c>
@@ -5967,12 +5633,12 @@
       <c r="D5" s="156">
         <v>0</v>
       </c>
-      <c r="E5" s="250"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="245"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="218"/>
     </row>
-    <row r="7" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="218"/>
     </row>
   </sheetData>
@@ -5997,15 +5663,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="155" t="s">
         <v>74</v>
@@ -6016,11 +5682,11 @@
       <c r="D1" s="155" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="250" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="245" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
@@ -6033,11 +5699,11 @@
       <c r="D2" s="156">
         <v>0</v>
       </c>
-      <c r="E2" s="250"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="245"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="156">
         <v>1.5214285714285714E-3</v>
@@ -6048,11 +5714,11 @@
       <c r="D3" s="156">
         <v>0</v>
       </c>
-      <c r="E3" s="250"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="245"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="156">
         <v>1.3000000000000002E-4</v>
@@ -6063,9 +5729,9 @@
       <c r="D4" s="156">
         <v>0</v>
       </c>
-      <c r="E4" s="250"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="245"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
         <v>76</v>
       </c>
@@ -6078,7 +5744,7 @@
       <c r="D5" s="156">
         <v>3.1250000000000003E-7</v>
       </c>
-      <c r="E5" s="250"/>
+      <c r="E5" s="245"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6101,31 +5767,31 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="64.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="64.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="155" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" s="155" t="s">
         <v>72</v>
       </c>
       <c r="D1" s="155" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="155" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="155" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
@@ -6139,12 +5805,12 @@
       <c r="D2" s="158"/>
       <c r="E2" s="158"/>
       <c r="F2" s="233" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="156">
         <v>2.07E-2</v>
@@ -6156,9 +5822,9 @@
       <c r="E3" s="158"/>
       <c r="F3" s="233"/>
     </row>
-    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="156">
         <v>2.07E-2</v>
@@ -6170,7 +5836,7 @@
       <c r="E4" s="158"/>
       <c r="F4" s="233"/>
     </row>
-    <row r="5" spans="1:6" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="89" t="s">
         <v>76</v>
       </c>
@@ -6199,24 +5865,24 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="62" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="62" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="62" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="62" customWidth="1"/>
     <col min="3" max="3" width="13" style="62" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="62" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="62" customWidth="1"/>
     <col min="6" max="6" width="14" style="62" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="62" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="62" customWidth="1"/>
     <col min="8" max="8" width="13" style="62" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="62" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="62"/>
+    <col min="9" max="9" width="14.5546875" style="62" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="258" t="s">
         <v>73</v>
@@ -6224,12 +5890,12 @@
       <c r="C1" s="259"/>
       <c r="D1" s="260"/>
       <c r="E1" s="258" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F1" s="259"/>
       <c r="G1" s="260"/>
       <c r="H1" s="258" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I1" s="259"/>
       <c r="J1" s="260"/>
@@ -6239,7 +5905,7 @@
       <c r="L1" s="259"/>
       <c r="M1" s="260"/>
     </row>
-    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
       <c r="B2" s="199" t="s">
         <v>77</v>
@@ -6278,7 +5944,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>74</v>
       </c>
@@ -6319,7 +5985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>75</v>
       </c>
@@ -6360,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>80</v>
       </c>
@@ -6401,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>81</v>
       </c>
@@ -6442,7 +6108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>82</v>
       </c>
@@ -6483,7 +6149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>83</v>
       </c>
@@ -6524,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="150" t="s">
         <v>84</v>
       </c>
@@ -6565,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="150" t="s">
         <v>85</v>
       </c>
@@ -6606,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="198" t="s">
         <v>86</v>
       </c>
@@ -6647,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="160" t="s">
         <v>18</v>
       </c>
@@ -6901,127 +6567,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="96" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="96" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="95" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="69" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="69" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="227" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="228" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="226" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="225" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="221" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="220" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="222" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="223" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="224" t="s">
-        <v>273</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="73" priority="6">
-      <formula>$B$2 = FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="NA">
-      <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Inf">
-      <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="70" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="69" priority="1">
-      <formula>$B$11&lt;&gt;"naive"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -7032,65 +6577,65 @@
       <selection activeCell="I3" sqref="I3:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="4.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="1" customWidth="1"/>
-    <col min="16" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="12.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="12.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="1" customWidth="1"/>
-    <col min="27" max="28" width="12.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="15.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="12.5703125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.42578125" style="1" customWidth="1"/>
-    <col min="35" max="36" width="8.85546875" style="1"/>
-    <col min="37" max="37" width="14.85546875" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.85546875" style="1"/>
+    <col min="16" max="17" width="4.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.44140625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="12.88671875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" style="1" customWidth="1"/>
+    <col min="23" max="24" width="12.44140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="1" customWidth="1"/>
+    <col min="27" max="28" width="12.5546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.44140625" style="1" customWidth="1"/>
+    <col min="31" max="32" width="12.5546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" style="1" customWidth="1"/>
+    <col min="35" max="36" width="8.88671875" style="1"/>
+    <col min="37" max="37" width="14.88671875" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S2" s="240" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="240"/>
-      <c r="U2" s="240"/>
-      <c r="V2" s="240"/>
-      <c r="W2" s="240" t="s">
+    <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="235" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="235"/>
+      <c r="U2" s="235"/>
+      <c r="V2" s="235"/>
+      <c r="W2" s="235" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="240"/>
-      <c r="Y2" s="240"/>
-      <c r="Z2" s="240"/>
-      <c r="AA2" s="240" t="s">
+      <c r="X2" s="235"/>
+      <c r="Y2" s="235"/>
+      <c r="Z2" s="235"/>
+      <c r="AA2" s="235" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="240"/>
-      <c r="AC2" s="240"/>
-      <c r="AD2" s="240"/>
-      <c r="AE2" s="240" t="s">
+      <c r="AB2" s="235"/>
+      <c r="AC2" s="235"/>
+      <c r="AD2" s="235"/>
+      <c r="AE2" s="235" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="240"/>
-      <c r="AG2" s="240"/>
-      <c r="AH2" s="240"/>
+      <c r="AF2" s="235"/>
+      <c r="AG2" s="235"/>
+      <c r="AH2" s="235"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -7104,7 +6649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
@@ -7218,7 +6763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -7313,7 +6858,7 @@
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
     </row>
-    <row r="5" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B5" s="20" t="s">
         <v>33</v>
       </c>
@@ -7436,7 +6981,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
@@ -7560,7 +7105,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B7" s="20" t="s">
         <v>42</v>
       </c>
@@ -7675,7 +7220,7 @@
       <c r="AM7" s="27"/>
       <c r="AN7" s="27"/>
     </row>
-    <row r="8" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
@@ -7787,7 +7332,7 @@
       </c>
       <c r="AJ8" s="87"/>
     </row>
-    <row r="9" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="I9" s="35" t="s">
         <v>45</v>
       </c>
@@ -7877,7 +7422,7 @@
       </c>
       <c r="AJ9" s="87"/>
     </row>
-    <row r="10" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I10" s="35" t="s">
         <v>46</v>
       </c>
@@ -7962,7 +7507,7 @@
       </c>
       <c r="AJ10" s="87"/>
     </row>
-    <row r="11" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I11" s="35" t="s">
         <v>47</v>
       </c>
@@ -8048,7 +7593,7 @@
       </c>
       <c r="AJ11" s="87"/>
     </row>
-    <row r="12" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I12" s="35" t="s">
         <v>48</v>
       </c>
@@ -8134,7 +7679,7 @@
       </c>
       <c r="AJ12" s="87"/>
     </row>
-    <row r="13" spans="2:40" ht="21.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:40" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="B13" s="61" t="s">
         <v>49</v>
       </c>
@@ -8230,7 +7775,7 @@
       </c>
       <c r="AJ13" s="87"/>
     </row>
-    <row r="14" spans="2:40" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:40" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="31"/>
       <c r="E14" s="34"/>
       <c r="I14" s="29" t="s">
@@ -8320,7 +7865,7 @@
       </c>
       <c r="AJ14" s="87"/>
     </row>
-    <row r="15" spans="2:40" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:40" ht="18" x14ac:dyDescent="0.3">
       <c r="B15" s="31"/>
       <c r="E15" s="34"/>
       <c r="I15" s="29" t="s">
@@ -8412,7 +7957,7 @@
       </c>
       <c r="AJ15" s="87"/>
     </row>
-    <row r="16" spans="2:40" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:40" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
@@ -8520,7 +8065,7 @@
       </c>
       <c r="AJ16" s="87"/>
     </row>
-    <row r="17" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
         <v>33</v>
       </c>
@@ -8543,10 +8088,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="241" t="s">
+      <c r="J17" s="236" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="244" t="s">
+      <c r="K17" s="239" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8622,7 +8167,7 @@
       </c>
       <c r="AJ17" s="27"/>
     </row>
-    <row r="18" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
         <v>1</v>
       </c>
@@ -8646,8 +8191,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="242"/>
-      <c r="K18" s="245"/>
+      <c r="J18" s="237"/>
+      <c r="K18" s="240"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8721,7 +8266,7 @@
       </c>
       <c r="AJ18" s="27"/>
     </row>
-    <row r="19" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
         <v>58</v>
       </c>
@@ -8745,8 +8290,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="242"/>
-      <c r="K19" s="245"/>
+      <c r="J19" s="237"/>
+      <c r="K19" s="240"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -8820,14 +8365,14 @@
       </c>
       <c r="AJ19" s="27"/>
     </row>
-    <row r="20" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="58"/>
       <c r="C20" s="58"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="242"/>
-      <c r="K20" s="245"/>
+      <c r="J20" s="237"/>
+      <c r="K20" s="240"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -8901,15 +8446,15 @@
       </c>
       <c r="AJ20" s="27"/>
     </row>
-    <row r="21" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="58"/>
       <c r="C21" s="58"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="242"/>
-      <c r="K21" s="245"/>
+      <c r="J21" s="237"/>
+      <c r="K21" s="240"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -8983,15 +8528,15 @@
       </c>
       <c r="AJ21" s="27"/>
     </row>
-    <row r="22" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="58"/>
       <c r="C22" s="58"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="242"/>
-      <c r="K22" s="245"/>
+      <c r="J22" s="237"/>
+      <c r="K22" s="240"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -9065,15 +8610,15 @@
       </c>
       <c r="AJ22" s="27"/>
     </row>
-    <row r="23" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="58"/>
       <c r="C23" s="58"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="242"/>
-      <c r="K23" s="245"/>
+      <c r="J23" s="237"/>
+      <c r="K23" s="240"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -9147,15 +8692,15 @@
       </c>
       <c r="AJ23" s="27"/>
     </row>
-    <row r="24" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="58"/>
       <c r="C24" s="58"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="242"/>
-      <c r="K24" s="245"/>
+      <c r="J24" s="237"/>
+      <c r="K24" s="240"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -9169,31 +8714,31 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
       <c r="C25" s="58"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="242"/>
-      <c r="K25" s="245"/>
-    </row>
-    <row r="26" spans="2:36" ht="18" x14ac:dyDescent="0.25">
+      <c r="J25" s="237"/>
+      <c r="K25" s="240"/>
+    </row>
+    <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
       <c r="C26" s="58"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="242"/>
-      <c r="K26" s="245"/>
-      <c r="N26" s="247" t="s">
+      <c r="J26" s="237"/>
+      <c r="K26" s="240"/>
+      <c r="N26" s="242" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="248"/>
-      <c r="P26" s="248"/>
-      <c r="Q26" s="249"/>
+      <c r="O26" s="243"/>
+      <c r="P26" s="243"/>
+      <c r="Q26" s="244"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -9262,21 +8807,21 @@
         <v>263.94800000000009</v>
       </c>
     </row>
-    <row r="27" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="58"/>
       <c r="C27" s="58"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="242"/>
-      <c r="K27" s="245"/>
-      <c r="N27" s="247" t="s">
+      <c r="J27" s="237"/>
+      <c r="K27" s="240"/>
+      <c r="N27" s="242" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="248"/>
-      <c r="P27" s="248"/>
-      <c r="Q27" s="249"/>
+      <c r="O27" s="243"/>
+      <c r="P27" s="243"/>
+      <c r="Q27" s="244"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -9345,46 +8890,46 @@
         <v>303.90184335522252</v>
       </c>
     </row>
-    <row r="28" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="58"/>
       <c r="C28" s="58"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="242"/>
-      <c r="K28" s="245"/>
+      <c r="J28" s="237"/>
+      <c r="K28" s="240"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
     </row>
-    <row r="29" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="242"/>
-      <c r="K29" s="245"/>
-    </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J30" s="242"/>
-      <c r="K30" s="245"/>
-    </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J31" s="242"/>
-      <c r="K31" s="245"/>
-    </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J32" s="242"/>
-      <c r="K32" s="245"/>
-    </row>
-    <row r="33" spans="10:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J33" s="243"/>
-      <c r="K33" s="246"/>
-    </row>
-    <row r="34" spans="10:26" x14ac:dyDescent="0.25">
+      <c r="J29" s="237"/>
+      <c r="K29" s="240"/>
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J30" s="237"/>
+      <c r="K30" s="240"/>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J31" s="237"/>
+      <c r="K31" s="240"/>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J32" s="237"/>
+      <c r="K32" s="240"/>
+    </row>
+    <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="238"/>
+      <c r="K33" s="241"/>
+    </row>
+    <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
       <c r="V34" s="65">
         <v>10</v>
@@ -9398,7 +8943,7 @@
       <c r="Y34"/>
       <c r="Z34"/>
     </row>
-    <row r="35" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U35" s="83" t="s">
         <v>68</v>
       </c>
@@ -9417,7 +8962,7 @@
       <c r="Y35"/>
       <c r="Z35"/>
     </row>
-    <row r="36" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U36" s="84" t="s">
         <v>69</v>
       </c>
@@ -9436,7 +8981,7 @@
       <c r="Y36"/>
       <c r="Z36"/>
     </row>
-    <row r="37" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U37" s="83" t="s">
         <v>70</v>
       </c>
@@ -9455,7 +9000,7 @@
       <c r="Y37"/>
       <c r="Z37"/>
     </row>
-    <row r="38" spans="10:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U38" s="85" t="s">
         <v>71</v>
       </c>
@@ -9474,7 +9019,7 @@
       <c r="Y38"/>
       <c r="Z38"/>
     </row>
-    <row r="39" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U39"/>
       <c r="V39"/>
       <c r="W39"/>
@@ -9494,82 +9039,82 @@
     <mergeCell ref="N27:Q27"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:AB7 AD5:AD7 AD9:AD16 S9:AB16">
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:AD23">
-    <cfRule type="cellIs" dxfId="67" priority="19" operator="notBetween">
+    <cfRule type="cellIs" dxfId="68" priority="19" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="20" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AB8 AD8">
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5:AC7 AC9:AC16">
-    <cfRule type="cellIs" dxfId="64" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="62" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5:AF7 AE9:AF16 AH9:AI16 AH5:AJ5 AH6:AI7 AJ6:AJ16 AH4">
-    <cfRule type="cellIs" dxfId="61" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AJ23">
-    <cfRule type="cellIs" dxfId="60" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="61" priority="9" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="10" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8 AH8:AI8">
-    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5:AG7 AG9:AG16">
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4 S4:AB4">
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4 AI4">
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9578,7 +9123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC80DB5-92D9-44E1-984F-05E418326CA4}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -9586,14 +9131,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="str">
         <f>Discretization!A15</f>
         <v>Dynamic dT</v>
@@ -9602,11 +9147,11 @@
         <f>Discretization!B15</f>
         <v>1</v>
       </c>
-      <c r="C1" s="250" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C1" s="245" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="str">
         <f>Parameters!A2</f>
         <v>Variable HRT</v>
@@ -9615,9 +9160,9 @@
         <f>Parameters!B2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="250"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C2" s="245"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
         <f>Bacteria!A6</f>
         <v>Initialisation method</v>
@@ -9626,9 +9171,9 @@
         <f>Bacteria!B6</f>
         <v>granule</v>
       </c>
-      <c r="C3" s="250"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C3" s="245"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
         <f>Bacteria!A12</f>
         <v>Inactivation enabled</v>
@@ -9637,9 +9182,9 @@
         <f>Bacteria!B12</f>
         <v>1</v>
       </c>
-      <c r="C4" s="250"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C4" s="245"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
         <f>Bacteria!A13</f>
         <v>Detachment method</v>
@@ -9648,9 +9193,9 @@
         <f>Bacteria!B13</f>
         <v>mechanistic</v>
       </c>
-      <c r="C5" s="250"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C5" s="245"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
         <f>Solver!A4</f>
         <v>pH bulk concentration corrected</v>
@@ -9659,9 +9204,9 @@
         <f>Solver!B4</f>
         <v>1</v>
       </c>
-      <c r="C6" s="250"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C6" s="245"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
         <f>Solver!A2</f>
         <v>pH solving included</v>
@@ -9670,9 +9215,9 @@
         <f>Solver!B2</f>
         <v>1</v>
       </c>
-      <c r="C7" s="250"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="245"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="str">
         <f>Solver!A5</f>
         <v>Speciation included</v>
@@ -9681,31 +9226,31 @@
         <f>Solver!B5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="250"/>
-    </row>
-    <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="245"/>
+    </row>
+    <row r="9" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="218"/>
       <c r="G9" s="217"/>
     </row>
-    <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="218"/>
       <c r="G10" s="217"/>
     </row>
-    <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="218"/>
       <c r="G11" s="217"/>
     </row>
-    <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="218"/>
       <c r="G12" s="217"/>
     </row>
-    <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="218"/>
     </row>
-    <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="218"/>
     </row>
-    <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="218"/>
     </row>
   </sheetData>
@@ -9716,24 +9261,495 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="66.88671875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="122">
+        <v>257</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="110" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="246" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="133">
+        <v>257</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="246"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="99">
+        <f>B5*B1*1000000</f>
+        <v>1028</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="246"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="99">
+        <f>B6*B2*1000000</f>
+        <v>1028</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="110" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="246"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="103">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="110" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="246"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="103">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="246"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="103">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="246"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="104">
+        <f>20*10^(-6)</f>
+        <v>1.9999999999999998E-5</v>
+      </c>
+      <c r="C8" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="247"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="105">
+        <v>6500</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="248" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="102">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="249"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="98">
+        <f>$B$5^2 * B10 / MAX(Diffusion!$B:$B)</f>
+        <v>6.0468631897203323E-7</v>
+      </c>
+      <c r="C11" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="110" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="249"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="249"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="106">
+        <v>24</v>
+      </c>
+      <c r="C13" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="110" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="249"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="100">
+        <f>24*7</f>
+        <v>168</v>
+      </c>
+      <c r="C14" s="124" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="250"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="107" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" s="134" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="125" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="113" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="248" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="102">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="114" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="249"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="98">
+        <f>$B$5^2 * B16 / MAX(Diffusion!$B:$B)</f>
+        <v>3.0234315948601663E-8</v>
+      </c>
+      <c r="C17" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="114" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="249"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="102">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="114" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="249"/>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="98">
+        <f>$B$5^2 * B18 / MAX(Diffusion!$B:$B)</f>
+        <v>1.511715797430083E-6</v>
+      </c>
+      <c r="C19" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="114" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="249"/>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="102">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="114" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="249"/>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="109">
+        <v>1</v>
+      </c>
+      <c r="C21" s="126" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="115" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="249"/>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="102">
+        <v>3</v>
+      </c>
+      <c r="C22" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="116" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="249"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="102">
+        <v>500</v>
+      </c>
+      <c r="C23" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="116" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="249"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="102">
+        <v>200</v>
+      </c>
+      <c r="C24" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="249"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="102">
+        <v>40</v>
+      </c>
+      <c r="C25" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="116" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="249"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="119">
+        <v>0.2</v>
+      </c>
+      <c r="C26" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="116" t="s">
+        <v>172</v>
+      </c>
+      <c r="E26" s="249"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="118">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C27" s="127" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="E27" s="249"/>
+    </row>
+    <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="120">
+        <v>0.02</v>
+      </c>
+      <c r="C28" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="117" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="250"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E1:E8"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="E15:E28"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A16:D28">
+    <cfRule type="expression" dxfId="53" priority="1">
+      <formula>$B$15 = FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{B02285CC-B93F-41B6-9F0B-F56D7F2E2904}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="62" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="62"/>
+    <col min="1" max="1" width="21.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="62" customWidth="1"/>
+    <col min="4" max="4" width="69.44140625" style="62" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>99</v>
       </c>
@@ -9748,7 +9764,7 @@
       </c>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>176</v>
       </c>
@@ -9763,7 +9779,7 @@
       </c>
       <c r="E2" s="69"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>179</v>
       </c>
@@ -9779,7 +9795,7 @@
       </c>
       <c r="E3" s="69"/>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="108" t="s">
         <v>180</v>
       </c>
@@ -9790,11 +9806,11 @@
         <v>97</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E4" s="69"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>39</v>
       </c>
@@ -9809,9 +9825,9 @@
       </c>
       <c r="E5" s="69"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="153">
         <f>B5+273.15</f>
@@ -9821,11 +9837,11 @@
         <v>41</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E6" s="69"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
         <v>175</v>
       </c>
@@ -9840,23 +9856,23 @@
       </c>
       <c r="E7" s="69"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="77" t="s">
         <v>174</v>
       </c>
       <c r="B8" s="128">
-        <f>(((Bacteria!B10/3)*Bacteria!B1)/3)/1000</f>
-        <v>2.3271056693257722E-10</v>
+        <f>B11/B12 * 4/3 * PI() *B10^3</f>
+        <v>1.3962634015954638E-7</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="110" t="s">
-        <v>184</v>
+        <v>281</v>
       </c>
       <c r="E8" s="69"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="77" t="s">
         <v>173</v>
       </c>
@@ -9865,122 +9881,147 @@
         <v>8.3143999999999996E-3</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" s="110" t="s">
         <v>173</v>
       </c>
       <c r="E9" s="69"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
+    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="220" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="158">
+        <f>1000*10^(-6)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="143" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="B11" s="261">
+        <v>100</v>
+      </c>
+      <c r="C11" s="90" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="116" t="s">
+        <v>286</v>
+      </c>
       <c r="E11" s="69"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="77" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="261">
+        <v>3</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="116" t="s">
+        <v>288</v>
+      </c>
       <c r="E12" s="69"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" s="94"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="69"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -10003,6 +10044,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10014,19 +10056,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="62"/>
+    <col min="1" max="1" width="9.109375" style="62"/>
     <col min="2" max="2" width="12" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="62" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="62" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="62"/>
-    <col min="7" max="7" width="11.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="62"/>
+    <col min="3" max="3" width="9.109375" style="62" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="62" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="62"/>
+    <col min="7" max="7" width="11.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
@@ -10038,13 +10080,13 @@
         <v>108</v>
       </c>
       <c r="D1" s="110" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="251" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="251" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
@@ -10056,11 +10098,11 @@
         <v>108</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="251"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
@@ -10072,11 +10114,11 @@
         <v>108</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="251"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
@@ -10088,11 +10130,11 @@
         <v>108</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E4" s="251"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
@@ -10104,11 +10146,11 @@
         <v>108</v>
       </c>
       <c r="D5" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5" s="251"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>83</v>
       </c>
@@ -10120,11 +10162,11 @@
         <v>108</v>
       </c>
       <c r="D6" s="110" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="251"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
         <v>84</v>
       </c>
@@ -10136,7 +10178,7 @@
         <v>108</v>
       </c>
       <c r="D7" s="111" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="252"/>
     </row>
@@ -10153,23 +10195,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="62" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="79.7109375" style="62" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="37.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="62" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="79.6640625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="98">
         <f>((4/3)*PI()*B3^3)*B4</f>
@@ -10179,12 +10221,12 @@
         <v>16</v>
       </c>
       <c r="D1" s="130" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="98">
         <f>0.1*B1</f>
@@ -10194,12 +10236,12 @@
         <v>16</v>
       </c>
       <c r="D2" s="130" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="131">
         <f>(1)*10^(-6)</f>
@@ -10209,12 +10251,12 @@
         <v>94</v>
       </c>
       <c r="D3" s="130" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="131">
         <f>500*1000</f>
@@ -10224,12 +10266,12 @@
         <v>95</v>
       </c>
       <c r="D4" s="130" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="137">
         <v>24.6</v>
@@ -10238,56 +10280,56 @@
         <v>96</v>
       </c>
       <c r="D5" s="130" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="138" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="142" t="s">
         <v>221</v>
-      </c>
-      <c r="B6" s="142" t="s">
-        <v>222</v>
       </c>
       <c r="C6" s="140" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="141" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="131">
-        <f>100*10^(-6)</f>
-        <v>9.9999999999999991E-5</v>
+        <f>25*10^(-6)</f>
+        <v>2.4999999999999998E-5</v>
       </c>
       <c r="C7" s="90" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="130" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B8" s="230">
         <f>_xlfn.CEILING.MATH(B7^2 / (0.8*B3 * B11)^2 * 0.75)</f>
-        <v>5209</v>
+        <v>326</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="130" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B9" s="229">
         <v>500</v>
@@ -10296,12 +10338,12 @@
         <v>97</v>
       </c>
       <c r="D9" s="136" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="131">
         <f>4*ROUND(((B15/2)^2)/((B3)^2),0)</f>
@@ -10311,10 +10353,10 @@
         <v>97</v>
       </c>
       <c r="D10" s="130" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>118</v>
       </c>
@@ -10325,12 +10367,12 @@
         <v>97</v>
       </c>
       <c r="D11" s="130" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
-        <v>205</v>
       </c>
       <c r="B12" s="137" t="b">
         <v>1</v>
@@ -10339,40 +10381,40 @@
         <v>97</v>
       </c>
       <c r="D12" s="130" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="138" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="138" t="s">
-        <v>207</v>
-      </c>
       <c r="B13" s="139" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C13" s="140" t="s">
         <v>97</v>
       </c>
       <c r="D13" s="141" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="132">
         <v>5</v>
       </c>
       <c r="C14" s="90" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D14" s="130" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A15" s="108" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="135">
         <f>1000*10^(-6)</f>
@@ -10382,26 +10424,26 @@
         <v>94</v>
       </c>
       <c r="D15" s="136" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="69"/>
       <c r="B16" s="94"/>
       <c r="C16" s="69"/>
       <c r="D16" s="69"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="94"/>
       <c r="D18" s="69"/>
       <c r="E18" s="69"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="69"/>
       <c r="D19" s="94"/>
       <c r="E19" s="69"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="69"/>
       <c r="D20" s="69"/>
       <c r="E20" s="94"/>
@@ -10448,32 +10490,32 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="131">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-8</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
       <c r="D1" s="130" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" s="132" t="b">
         <v>1</v>
@@ -10482,12 +10524,12 @@
         <v>97</v>
       </c>
       <c r="D2" s="130" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" s="131">
         <v>1.0000000000000001E-15</v>
@@ -10496,12 +10538,12 @@
         <v>97</v>
       </c>
       <c r="D3" s="130" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" s="132" t="b">
         <v>1</v>
@@ -10510,12 +10552,12 @@
         <v>97</v>
       </c>
       <c r="D4" s="130" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5" s="132" t="b">
         <v>1</v>
@@ -10524,12 +10566,12 @@
         <v>97</v>
       </c>
       <c r="D5" s="130" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="131">
         <v>1E-8</v>
@@ -10538,12 +10580,12 @@
         <v>97</v>
       </c>
       <c r="D6" s="130" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="234">
         <v>5.0000000000000001E-4</v>
@@ -10552,26 +10594,26 @@
         <v>109</v>
       </c>
       <c r="D7" s="130" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="132" t="s">
         <v>213</v>
-      </c>
-      <c r="B8" s="132" t="s">
-        <v>214</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="130" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9" s="132">
         <v>2</v>
@@ -10580,12 +10622,12 @@
         <v>97</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10" s="229" t="b">
         <v>0</v>
@@ -10594,12 +10636,12 @@
         <v>97</v>
       </c>
       <c r="D10" s="232" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="132" t="b">
         <v>0</v>
@@ -10608,12 +10650,12 @@
         <v>97</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" s="132" t="s">
         <v>113</v>
@@ -10622,7 +10664,7 @@
         <v>97</v>
       </c>
       <c r="D12" s="143" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -10653,157 +10695,194 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="62"/>
-    <col min="3" max="3" width="7.5703125" style="62" customWidth="1"/>
-    <col min="4" max="4" width="75.42578125" style="62" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="62"/>
-    <col min="7" max="7" width="12" style="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="62"/>
+    <col min="1" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="4.44140625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="62.5546875" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="131">
-        <v>9.9999999999999995E-7</v>
+        <f>40/(17*1000)</f>
+        <v>2.352941176470588E-3</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="253" t="s">
+      <c r="D1" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="253" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="69"/>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="131">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="253"/>
-      <c r="E2" s="69"/>
+      <c r="D2" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="253"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="253"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="253"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="131">
-        <f>Influent!B4</f>
+        <f>6/(32*1000)</f>
         <v>1.875E-4</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="253"/>
-      <c r="E4" s="69"/>
+      <c r="D4" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="253"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="131">
-        <f>Influent!B5</f>
         <v>1E-3</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="253"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="D5" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="253"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="69"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="108" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="135">
+      <c r="B6" s="131">
         <f>B1/2</f>
-        <v>4.9999999999999998E-7</v>
-      </c>
-      <c r="C6" s="126" t="s">
+        <v>1.176470588235294E-3</v>
+      </c>
+      <c r="C6" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="D6" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="253"/>
+      <c r="F6" s="94"/>
       <c r="G6" s="69"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="150" t="s">
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="151">
+      <c r="B7" s="131">
         <f>B5</f>
         <v>1E-3</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="253"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="146"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E8" s="69"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="147"/>
-      <c r="J8" s="146"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="94"/>
+      <c r="D7" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="253"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:D7"/>
+    <mergeCell ref="E1:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
README and other stuff
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMX.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\IbM\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06BD545-A891-4A6E-971D-16A763FBCACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703E0955-D481-4137-9070-6DB7D852585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Chiel:</t>
         </r>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 based on Poot et al (2016)</t>
@@ -1531,7 +1531,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1759,6 +1759,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1805,19 +1806,6 @@
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3628,6 +3616,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="41" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3706,7 +3695,6 @@
     <xf numFmtId="0" fontId="24" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4489,8 +4477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4635,7 +4623,7 @@
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="257" t="s">
+      <c r="D1" s="258" t="s">
         <v>225</v>
       </c>
       <c r="E1" s="69"/>
@@ -4652,7 +4640,7 @@
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="257"/>
+      <c r="D2" s="258"/>
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
@@ -4667,7 +4655,7 @@
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="257"/>
+      <c r="D3" s="258"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
@@ -4683,7 +4671,7 @@
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="257"/>
+      <c r="D4" s="258"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
@@ -4699,7 +4687,7 @@
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="257"/>
+      <c r="D5" s="258"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
@@ -4715,7 +4703,7 @@
       <c r="C6" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="257"/>
+      <c r="D6" s="258"/>
       <c r="E6" s="69"/>
       <c r="F6" s="69"/>
       <c r="G6" s="69"/>
@@ -4731,7 +4719,7 @@
       <c r="C7" s="150" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="257"/>
+      <c r="D7" s="258"/>
       <c r="E7" s="69"/>
       <c r="F7" s="143"/>
       <c r="G7" s="143"/>
@@ -4830,7 +4818,7 @@
       <c r="H2" s="162" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="257" t="s">
+      <c r="I2" s="258" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4859,7 +4847,7 @@
       <c r="H3" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="257"/>
+      <c r="I3" s="258"/>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
@@ -4886,7 +4874,7 @@
       <c r="H4" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="257"/>
+      <c r="I4" s="258"/>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
@@ -4913,7 +4901,7 @@
       <c r="H5" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="257"/>
+      <c r="I5" s="258"/>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
@@ -4941,7 +4929,7 @@
       <c r="H6" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="257"/>
+      <c r="I6" s="258"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
@@ -4970,7 +4958,7 @@
       <c r="H7" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="257"/>
+      <c r="I7" s="258"/>
     </row>
     <row r="8" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="148" t="s">
@@ -4997,7 +4985,7 @@
       <c r="H8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="257"/>
+      <c r="I8" s="258"/>
     </row>
     <row r="9" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
@@ -5024,7 +5012,7 @@
       <c r="H9" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="257"/>
+      <c r="I9" s="258"/>
     </row>
     <row r="10" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="157" t="s">
@@ -5051,7 +5039,7 @@
       <c r="H10" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="257"/>
+      <c r="I10" s="258"/>
     </row>
     <row r="11" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="158" t="s">
@@ -5078,7 +5066,7 @@
       <c r="H11" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="257"/>
+      <c r="I11" s="258"/>
     </row>
     <row r="12" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="159" t="s">
@@ -5119,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="256" t="s">
+      <c r="I13" s="257" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5144,7 +5132,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="256"/>
+      <c r="I14" s="257"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
@@ -5167,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="256"/>
+      <c r="I15" s="257"/>
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
@@ -5190,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="256"/>
+      <c r="I16" s="257"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
@@ -5213,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="256"/>
+      <c r="I17" s="257"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="108" t="s">
@@ -5236,7 +5224,7 @@
       </c>
       <c r="F18" s="71"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="256"/>
+      <c r="I18" s="257"/>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="148" t="s">
@@ -5260,7 +5248,7 @@
       </c>
       <c r="F19" s="71"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="256"/>
+      <c r="I19" s="257"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="148" t="s">
@@ -5284,7 +5272,7 @@
       </c>
       <c r="F20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="256"/>
+      <c r="I20" s="257"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="157" t="s">
@@ -5308,7 +5296,7 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="256"/>
+      <c r="I21" s="257"/>
     </row>
     <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="158" t="s">
@@ -5331,17 +5319,17 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="256"/>
+      <c r="I22" s="257"/>
     </row>
     <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="258" t="s">
+      <c r="A23" s="259" t="s">
         <v>232</v>
       </c>
-      <c r="B23" s="259"/>
-      <c r="C23" s="259"/>
-      <c r="D23" s="259"/>
-      <c r="E23" s="259"/>
-      <c r="F23" s="260"/>
+      <c r="B23" s="260"/>
+      <c r="C23" s="260"/>
+      <c r="D23" s="260"/>
+      <c r="E23" s="260"/>
+      <c r="F23" s="261"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -5362,7 +5350,7 @@
       <c r="F24" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="256" t="s">
+      <c r="I24" s="257" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5385,7 +5373,7 @@
       <c r="F25" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="256"/>
+      <c r="I25" s="257"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
@@ -5406,7 +5394,7 @@
       <c r="F26" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="256"/>
+      <c r="I26" s="257"/>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
@@ -5427,7 +5415,7 @@
       <c r="F27" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="256"/>
+      <c r="I27" s="257"/>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
@@ -5448,7 +5436,7 @@
       <c r="F28" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="256"/>
+      <c r="I28" s="257"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
@@ -5469,7 +5457,7 @@
       <c r="F29" s="185" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="256"/>
+      <c r="I29" s="257"/>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="148" t="s">
@@ -5490,7 +5478,7 @@
       <c r="F30" s="189" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="256"/>
+      <c r="I30" s="257"/>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="148" t="s">
@@ -5511,7 +5499,7 @@
       <c r="F31" s="187" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="256"/>
+      <c r="I31" s="257"/>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="157" t="s">
@@ -5532,7 +5520,7 @@
       <c r="F32" s="183" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="256"/>
+      <c r="I32" s="257"/>
     </row>
     <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="158" t="s">
@@ -5553,7 +5541,7 @@
       <c r="F33" s="172" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="256"/>
+      <c r="I33" s="257"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5609,7 +5597,7 @@
       <c r="D1" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="248" t="s">
+      <c r="E1" s="249" t="s">
         <v>244</v>
       </c>
     </row>
@@ -5626,7 +5614,7 @@
       <c r="D2" s="154">
         <v>3.5937500000000001E-6</v>
       </c>
-      <c r="E2" s="248"/>
+      <c r="E2" s="249"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5641,7 +5629,7 @@
       <c r="D3" s="154">
         <v>2.5937500000000004E-6</v>
       </c>
-      <c r="E3" s="248"/>
+      <c r="E3" s="249"/>
     </row>
     <row r="4" spans="1:5" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5656,7 +5644,7 @@
       <c r="D4" s="154">
         <v>0</v>
       </c>
-      <c r="E4" s="248"/>
+      <c r="E4" s="249"/>
     </row>
     <row r="5" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="216"/>
@@ -5705,7 +5693,7 @@
       <c r="D1" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="248" t="s">
+      <c r="E1" s="249" t="s">
         <v>243</v>
       </c>
     </row>
@@ -5722,7 +5710,7 @@
       <c r="D2" s="154">
         <v>0</v>
       </c>
-      <c r="E2" s="248"/>
+      <c r="E2" s="249"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5737,7 +5725,7 @@
       <c r="D3" s="154">
         <v>0</v>
       </c>
-      <c r="E3" s="248"/>
+      <c r="E3" s="249"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5752,7 +5740,7 @@
       <c r="D4" s="154">
         <v>3.1250000000000003E-7</v>
       </c>
-      <c r="E4" s="248"/>
+      <c r="E4" s="249"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5798,7 +5786,7 @@
       <c r="E1" s="153" t="s">
         <v>241</v>
       </c>
-      <c r="F1" s="257" t="s">
+      <c r="F1" s="258" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5815,7 +5803,7 @@
       </c>
       <c r="D2" s="156"/>
       <c r="E2" s="156"/>
-      <c r="F2" s="257"/>
+      <c r="F2" s="258"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5829,7 +5817,7 @@
       </c>
       <c r="D3" s="156"/>
       <c r="E3" s="156"/>
-      <c r="F3" s="257"/>
+      <c r="F3" s="258"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5844,7 +5832,7 @@
       </c>
       <c r="D4" s="156"/>
       <c r="E4" s="156"/>
-      <c r="F4" s="257"/>
+      <c r="F4" s="258"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5879,21 +5867,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
-      <c r="B1" s="261" t="s">
+      <c r="B1" s="262" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="262"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="261" t="s">
+      <c r="C1" s="263"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="262" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="262"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="262" t="s">
+      <c r="F1" s="263"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="263" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="262"/>
-      <c r="J1" s="263"/>
+      <c r="I1" s="263"/>
+      <c r="J1" s="264"/>
     </row>
     <row r="2" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
@@ -6462,30 +6450,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="S2" s="238" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="238"/>
-      <c r="U2" s="238"/>
-      <c r="V2" s="238"/>
-      <c r="W2" s="238" t="s">
+      <c r="S2" s="239" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="239"/>
+      <c r="U2" s="239"/>
+      <c r="V2" s="239"/>
+      <c r="W2" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="238"/>
-      <c r="Y2" s="238"/>
-      <c r="Z2" s="238"/>
-      <c r="AA2" s="238" t="s">
+      <c r="X2" s="239"/>
+      <c r="Y2" s="239"/>
+      <c r="Z2" s="239"/>
+      <c r="AA2" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="238"/>
-      <c r="AC2" s="238"/>
-      <c r="AD2" s="238"/>
-      <c r="AE2" s="238" t="s">
+      <c r="AB2" s="239"/>
+      <c r="AC2" s="239"/>
+      <c r="AD2" s="239"/>
+      <c r="AE2" s="239" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="238"/>
-      <c r="AG2" s="238"/>
-      <c r="AH2" s="238"/>
+      <c r="AF2" s="239"/>
+      <c r="AG2" s="239"/>
+      <c r="AH2" s="239"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -7938,10 +7926,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="239" t="s">
+      <c r="J17" s="240" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="242" t="s">
+      <c r="K17" s="243" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8041,8 +8029,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="240"/>
-      <c r="K18" s="243"/>
+      <c r="J18" s="241"/>
+      <c r="K18" s="244"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8140,8 +8128,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="240"/>
-      <c r="K19" s="243"/>
+      <c r="J19" s="241"/>
+      <c r="K19" s="244"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -8221,8 +8209,8 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="243"/>
+      <c r="J20" s="241"/>
+      <c r="K20" s="244"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -8303,8 +8291,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="243"/>
+      <c r="J21" s="241"/>
+      <c r="K21" s="244"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -8385,8 +8373,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="240"/>
-      <c r="K22" s="243"/>
+      <c r="J22" s="241"/>
+      <c r="K22" s="244"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -8467,8 +8455,8 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="240"/>
-      <c r="K23" s="243"/>
+      <c r="J23" s="241"/>
+      <c r="K23" s="244"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -8549,8 +8537,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="240"/>
-      <c r="K24" s="243"/>
+      <c r="J24" s="241"/>
+      <c r="K24" s="244"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -8571,8 +8559,8 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="240"/>
-      <c r="K25" s="243"/>
+      <c r="J25" s="241"/>
+      <c r="K25" s="244"/>
     </row>
     <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
@@ -8581,14 +8569,14 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="243"/>
-      <c r="N26" s="245" t="s">
+      <c r="J26" s="241"/>
+      <c r="K26" s="244"/>
+      <c r="N26" s="246" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="246"/>
-      <c r="P26" s="246"/>
-      <c r="Q26" s="247"/>
+      <c r="O26" s="247"/>
+      <c r="P26" s="247"/>
+      <c r="Q26" s="248"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -8664,14 +8652,14 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="240"/>
-      <c r="K27" s="243"/>
-      <c r="N27" s="245" t="s">
+      <c r="J27" s="241"/>
+      <c r="K27" s="244"/>
+      <c r="N27" s="246" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="246"/>
-      <c r="P27" s="246"/>
-      <c r="Q27" s="247"/>
+      <c r="O27" s="247"/>
+      <c r="P27" s="247"/>
+      <c r="Q27" s="248"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -8747,8 +8735,8 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="240"/>
-      <c r="K28" s="243"/>
+      <c r="J28" s="241"/>
+      <c r="K28" s="244"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
@@ -8760,24 +8748,24 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="240"/>
-      <c r="K29" s="243"/>
+      <c r="J29" s="241"/>
+      <c r="K29" s="244"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J30" s="240"/>
-      <c r="K30" s="243"/>
+      <c r="J30" s="241"/>
+      <c r="K30" s="244"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J31" s="240"/>
-      <c r="K31" s="243"/>
+      <c r="J31" s="241"/>
+      <c r="K31" s="244"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J32" s="240"/>
-      <c r="K32" s="243"/>
+      <c r="J32" s="241"/>
+      <c r="K32" s="244"/>
     </row>
     <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J33" s="241"/>
-      <c r="K33" s="244"/>
+      <c r="J33" s="242"/>
+      <c r="K33" s="245"/>
     </row>
     <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
@@ -8997,7 +8985,7 @@
         <f>Discretization!B15</f>
         <v>1</v>
       </c>
-      <c r="C1" s="248" t="s">
+      <c r="C1" s="249" t="s">
         <v>256</v>
       </c>
     </row>
@@ -9010,7 +8998,7 @@
         <f>Parameters!B2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="248"/>
+      <c r="C2" s="249"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
@@ -9021,7 +9009,7 @@
         <f>Bacteria!B6</f>
         <v>granule</v>
       </c>
-      <c r="C3" s="248"/>
+      <c r="C3" s="249"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
@@ -9032,7 +9020,7 @@
         <f>Bacteria!B12</f>
         <v>1.5</v>
       </c>
-      <c r="C4" s="248"/>
+      <c r="C4" s="249"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
@@ -9043,7 +9031,7 @@
         <f>Bacteria!B13</f>
         <v>1</v>
       </c>
-      <c r="C5" s="248"/>
+      <c r="C5" s="249"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
@@ -9054,7 +9042,7 @@
         <f>Solver!B4</f>
         <v>1</v>
       </c>
-      <c r="C6" s="248"/>
+      <c r="C6" s="249"/>
     </row>
     <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
@@ -9065,7 +9053,7 @@
         <f>Solver!B2</f>
         <v>1</v>
       </c>
-      <c r="C7" s="248"/>
+      <c r="C7" s="249"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="str">
@@ -9076,7 +9064,7 @@
         <f>Solver!B5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="248"/>
+      <c r="C8" s="249"/>
     </row>
     <row r="9" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="216"/>
@@ -9141,7 +9129,7 @@
       <c r="D1" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="249" t="s">
+      <c r="E1" s="250" t="s">
         <v>134</v>
       </c>
     </row>
@@ -9158,7 +9146,7 @@
       <c r="D2" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="249"/>
+      <c r="E2" s="250"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -9174,7 +9162,7 @@
       <c r="D3" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="249"/>
+      <c r="E3" s="250"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -9190,7 +9178,7 @@
       <c r="D4" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="249"/>
+      <c r="E4" s="250"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -9205,7 +9193,7 @@
       <c r="D5" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="249"/>
+      <c r="E5" s="250"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -9220,7 +9208,7 @@
       <c r="D6" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="249"/>
+      <c r="E6" s="250"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
@@ -9236,7 +9224,7 @@
       <c r="D7" s="110" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="249"/>
+      <c r="E7" s="250"/>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
@@ -9252,7 +9240,7 @@
       <c r="D8" s="111" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="250"/>
+      <c r="E8" s="251"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
@@ -9267,7 +9255,7 @@
       <c r="D9" s="112" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="251" t="s">
+      <c r="E9" s="252" t="s">
         <v>135</v>
       </c>
     </row>
@@ -9284,7 +9272,7 @@
       <c r="D10" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="E10" s="252"/>
+      <c r="E10" s="253"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
@@ -9300,7 +9288,7 @@
       <c r="D11" s="110" t="s">
         <v>147</v>
       </c>
-      <c r="E11" s="252"/>
+      <c r="E11" s="253"/>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
@@ -9315,7 +9303,7 @@
       <c r="D12" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="252"/>
+      <c r="E12" s="253"/>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
@@ -9331,7 +9319,7 @@
       <c r="D13" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="252"/>
+      <c r="E13" s="253"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
@@ -9347,7 +9335,7 @@
       <c r="D14" s="111" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="253"/>
+      <c r="E14" s="254"/>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="107" t="s">
@@ -9362,7 +9350,7 @@
       <c r="D15" s="113" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="251" t="s">
+      <c r="E15" s="252" t="s">
         <v>168</v>
       </c>
     </row>
@@ -9379,7 +9367,7 @@
       <c r="D16" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="252"/>
+      <c r="E16" s="253"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="77" t="s">
@@ -9395,7 +9383,7 @@
       <c r="D17" s="114" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="252"/>
+      <c r="E17" s="253"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
@@ -9410,7 +9398,7 @@
       <c r="D18" s="114" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="252"/>
+      <c r="E18" s="253"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
@@ -9426,7 +9414,7 @@
       <c r="D19" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="E19" s="252"/>
+      <c r="E19" s="253"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
@@ -9441,7 +9429,7 @@
       <c r="D20" s="114" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="252"/>
+      <c r="E20" s="253"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="108" t="s">
@@ -9456,7 +9444,7 @@
       <c r="D21" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="E21" s="252"/>
+      <c r="E21" s="253"/>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
@@ -9471,7 +9459,7 @@
       <c r="D22" s="116" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="252"/>
+      <c r="E22" s="253"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
@@ -9486,7 +9474,7 @@
       <c r="D23" s="116" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="252"/>
+      <c r="E23" s="253"/>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
@@ -9501,7 +9489,7 @@
       <c r="D24" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="252"/>
+      <c r="E24" s="253"/>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
@@ -9516,7 +9504,7 @@
       <c r="D25" s="116" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="252"/>
+      <c r="E25" s="253"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
@@ -9531,7 +9519,7 @@
       <c r="D26" s="116" t="s">
         <v>287</v>
       </c>
-      <c r="E26" s="252"/>
+      <c r="E26" s="253"/>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="77" t="s">
@@ -9546,7 +9534,7 @@
       <c r="D27" s="116" t="s">
         <v>283</v>
       </c>
-      <c r="E27" s="252"/>
+      <c r="E27" s="253"/>
     </row>
     <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="89" t="s">
@@ -9561,7 +9549,7 @@
       <c r="D28" s="117" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="253"/>
+      <c r="E28" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9811,7 +9799,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17"/>
-      <c r="B17" s="264">
+      <c r="B17" s="238">
         <f>4/3 * PI() *B10^3</f>
         <v>1.4137166941154065E-11</v>
       </c>
@@ -9937,7 +9925,7 @@
       <c r="D1" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="254" t="s">
+      <c r="E1" s="255" t="s">
         <v>181</v>
       </c>
     </row>
@@ -9955,7 +9943,7 @@
       <c r="D2" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E2" s="254"/>
+      <c r="E2" s="255"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -9971,7 +9959,7 @@
       <c r="D3" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="254"/>
+      <c r="E3" s="255"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -9987,7 +9975,7 @@
       <c r="D4" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="254"/>
+      <c r="E4" s="255"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -10003,7 +9991,7 @@
       <c r="D5" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E5" s="254"/>
+      <c r="E5" s="255"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -10019,7 +10007,7 @@
       <c r="D6" s="110" t="s">
         <v>180</v>
       </c>
-      <c r="E6" s="254"/>
+      <c r="E6" s="255"/>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
@@ -10035,7 +10023,7 @@
       <c r="D7" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="255"/>
+      <c r="E7" s="256"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10050,7 +10038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -10586,7 +10574,7 @@
       <c r="D1" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="256" t="s">
+      <c r="E1" s="257" t="s">
         <v>226</v>
       </c>
       <c r="F1" s="69"/>
@@ -10608,7 +10596,7 @@
       <c r="D2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="256"/>
+      <c r="E2" s="257"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
@@ -10628,7 +10616,7 @@
       <c r="D3" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="256"/>
+      <c r="E3" s="257"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
@@ -10649,7 +10637,7 @@
       <c r="D4" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="256"/>
+      <c r="E4" s="257"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
@@ -10669,7 +10657,7 @@
       <c r="D5" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="256"/>
+      <c r="E5" s="257"/>
       <c r="F5" s="94"/>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
@@ -10690,7 +10678,7 @@
       <c r="D6" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="256"/>
+      <c r="E6" s="257"/>
       <c r="F6" s="94"/>
       <c r="G6" s="69"/>
       <c r="H6" s="69"/>
@@ -10711,7 +10699,7 @@
       <c r="D7" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="256"/>
+      <c r="E7" s="257"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>

</xml_diff>